<commit_message>
Update data and HTML
</commit_message>
<xml_diff>
--- a/data/vintage_data/data_20010214.xlsx
+++ b/data/vintage_data/data_20010214.xlsx
@@ -16627,7 +16627,9 @@
       </c>
       <c r="W101" t="inlineStr"/>
       <c r="X101" t="inlineStr"/>
-      <c r="Y101" t="inlineStr"/>
+      <c r="Y101" t="n">
+        <v>4.2471</v>
+      </c>
       <c r="Z101" t="inlineStr"/>
     </row>
   </sheetData>
@@ -32955,7 +32957,9 @@
       </c>
       <c r="W101" t="inlineStr"/>
       <c r="X101" t="inlineStr"/>
-      <c r="Y101" t="inlineStr"/>
+      <c r="Y101" t="n">
+        <v>4.2471</v>
+      </c>
       <c r="Z101" t="inlineStr"/>
     </row>
   </sheetData>

</xml_diff>